<commit_message>
WIP: layout - new map colours, bootstrap v5
</commit_message>
<xml_diff>
--- a/src/lib/gen-generic/port-battle.xlsx
+++ b/src/lib/gen-generic/port-battle.xlsx
@@ -1373,7 +1373,7 @@
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <color rgb="00373b2b"/>
+      <color rgb="0029281a"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
@@ -1381,7 +1381,7 @@
     </font>
     <font>
       <b/>
-      <color rgb="0035c399"/>
+      <color rgb="003bad8b"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
@@ -1389,7 +1389,7 @@
     </font>
     <font>
       <b/>
-      <color rgb="00c9ccc1"/>
+      <color rgb="00e0e0d9"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
@@ -1397,7 +1397,7 @@
     </font>
     <font>
       <b/>
-      <color rgb="00373b2b"/>
+      <color rgb="0029281a"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
@@ -1413,32 +1413,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00c9ccc1"/>
+        <fgColor rgb="00e0e0d9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0082886f"/>
+        <fgColor rgb="00858468"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00b2b5a6"/>
+        <fgColor rgb="00c2c1b3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00e1e3dd"/>
+        <fgColor rgb="00f0f0ec"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00eeebe7"/>
+        <fgColor rgb="00f3f1ef"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00fdfdfd"/>
+        <fgColor rgb="00faf9f9"/>
       </patternFill>
     </fill>
   </fills>
@@ -1454,10 +1454,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color rgb="00b2b5a6"/>
+        <color rgb="00c2c1b3"/>
       </top>
       <bottom style="thin">
-        <color rgb="00b2b5a6"/>
+        <color rgb="00c2c1b3"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1515,7 +1515,7 @@
     <dxf>
       <font>
         <b/>
-        <color rgb="00cd4488"/>
+        <color rgb="00b5467d"/>
         <family val="2"/>
         <scheme val="minor"/>
         <sz val="14"/>
@@ -1525,7 +1525,7 @@
     <dxf>
       <font>
         <b/>
-        <color rgb="00cd4488"/>
+        <color rgb="00b5467d"/>
         <family val="2"/>
         <scheme val="minor"/>
         <sz val="14"/>

</xml_diff>